<commit_message>
Changed a few things so all numbers are '.' and not ','
</commit_message>
<xml_diff>
--- a/Sprungdaten_processed/class_std_mean.xlsx
+++ b/Sprungdaten_processed/class_std_mean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X51"/>
+  <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2308,70 +2308,70 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>14.85416666666667</v>
+        <v>14.811</v>
       </c>
       <c r="D25" t="n">
-        <v>14.68638888888889</v>
+        <v>14.7015</v>
       </c>
       <c r="E25" t="n">
-        <v>-3.885555555555556</v>
+        <v>-1.875375</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.5276111111111111</v>
+        <v>-0.6473749999999999</v>
       </c>
       <c r="G25" t="n">
-        <v>4.780166666666667</v>
+        <v>5.05025</v>
       </c>
       <c r="H25" t="n">
-        <v>4.871722222222222</v>
+        <v>8.1205</v>
       </c>
       <c r="I25" t="n">
-        <v>-103.4526111111111</v>
+        <v>-36.26512499999999</v>
       </c>
       <c r="J25" t="n">
-        <v>11.48588888888889</v>
+        <v>13.29325</v>
       </c>
       <c r="K25" t="n">
-        <v>8.303666666666667</v>
+        <v>13.04425</v>
       </c>
       <c r="L25" t="n">
-        <v>-183.2552222222222</v>
+        <v>-66.11762499999999</v>
       </c>
       <c r="M25" t="n">
-        <v>17.70605555555555</v>
+        <v>20.946125</v>
       </c>
       <c r="N25" t="n">
-        <v>27.54405555555556</v>
+        <v>34.19675</v>
       </c>
       <c r="O25" t="n">
-        <v>304.8005</v>
+        <v>304.482625</v>
       </c>
       <c r="P25" t="n">
-        <v>46.03177777777778</v>
+        <v>53.268125</v>
       </c>
       <c r="Q25" t="n">
-        <v>27.64738888888889</v>
+        <v>27.243875</v>
       </c>
       <c r="R25" t="n">
-        <v>23.23311111111111</v>
+        <v>23.109625</v>
       </c>
       <c r="S25" t="n">
-        <v>16.90227777777778</v>
+        <v>16.093875</v>
       </c>
       <c r="T25" t="n">
-        <v>1.644611111111111</v>
+        <v>1.971625</v>
       </c>
       <c r="U25" t="n">
-        <v>20.24066666666666</v>
+        <v>20.625375</v>
       </c>
       <c r="V25" t="n">
-        <v>12.91516666666667</v>
+        <v>13.86125</v>
       </c>
       <c r="W25" t="n">
-        <v>122.5273888888889</v>
+        <v>123.710125</v>
       </c>
       <c r="X25" t="n">
-        <v>20.08138888888889</v>
+        <v>23.838875</v>
       </c>
     </row>
     <row r="26">
@@ -2988,74 +2988,74 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Triffis C</t>
+          <t>3/4 Salto Vw A</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>45.26</v>
+        <v>14.8887</v>
       </c>
       <c r="D34" t="n">
-        <v>45.75</v>
+        <v>14.6743</v>
       </c>
       <c r="E34" t="n">
-        <v>-29.881</v>
+        <v>-5.4937</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.619</v>
+        <v>-0.4318</v>
       </c>
       <c r="G34" t="n">
-        <v>3.723</v>
+        <v>4.5641</v>
       </c>
       <c r="H34" t="n">
-        <v>-18.669</v>
+        <v>2.2727</v>
       </c>
       <c r="I34" t="n">
-        <v>-395.789</v>
+        <v>-157.2026</v>
       </c>
       <c r="J34" t="n">
-        <v>-82.48999999999999</v>
+        <v>10.04</v>
       </c>
       <c r="K34" t="n">
-        <v>-37.545</v>
+        <v>4.5112</v>
       </c>
       <c r="L34" t="n">
-        <v>-804.385</v>
+        <v>-276.9653</v>
       </c>
       <c r="M34" t="n">
-        <v>-167.241</v>
+        <v>15.114</v>
       </c>
       <c r="N34" t="n">
-        <v>88.51899999999999</v>
+        <v>22.2219</v>
       </c>
       <c r="O34" t="n">
-        <v>1057.916</v>
+        <v>305.0548</v>
       </c>
       <c r="P34" t="n">
-        <v>222.419</v>
+        <v>40.2427</v>
       </c>
       <c r="Q34" t="n">
-        <v>24.528</v>
+        <v>27.9702</v>
       </c>
       <c r="R34" t="n">
-        <v>22.774</v>
+        <v>23.3319</v>
       </c>
       <c r="S34" t="n">
-        <v>28.084</v>
+        <v>17.549</v>
       </c>
       <c r="T34" t="n">
-        <v>4.168</v>
+        <v>1.383</v>
       </c>
       <c r="U34" t="n">
-        <v>27.565</v>
+        <v>19.9329</v>
       </c>
       <c r="V34" t="n">
-        <v>52.83600000000001</v>
+        <v>12.1583</v>
       </c>
       <c r="W34" t="n">
-        <v>446.2619999999999</v>
+        <v>121.5812</v>
       </c>
       <c r="X34" t="n">
-        <v>160.213</v>
+        <v>17.0754</v>
       </c>
     </row>
     <row r="35">
@@ -3064,74 +3064,74 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1/2 ein 1/2 aus B</t>
+          <t>Triffis C</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>29.174</v>
+        <v>45.26</v>
       </c>
       <c r="D35" t="n">
-        <v>29.073</v>
+        <v>45.75</v>
       </c>
       <c r="E35" t="n">
-        <v>-9.818</v>
+        <v>-29.881</v>
       </c>
       <c r="F35" t="n">
-        <v>3.523</v>
+        <v>-0.619</v>
       </c>
       <c r="G35" t="n">
-        <v>1.067</v>
+        <v>3.723</v>
       </c>
       <c r="H35" t="n">
-        <v>-126.883</v>
+        <v>-18.669</v>
       </c>
       <c r="I35" t="n">
-        <v>-49.182</v>
+        <v>-395.789</v>
       </c>
       <c r="J35" t="n">
-        <v>-150.656</v>
+        <v>-82.48999999999999</v>
       </c>
       <c r="K35" t="n">
-        <v>-253.276</v>
+        <v>-37.545</v>
       </c>
       <c r="L35" t="n">
-        <v>-96.836</v>
+        <v>-804.385</v>
       </c>
       <c r="M35" t="n">
-        <v>-300.884</v>
+        <v>-167.241</v>
       </c>
       <c r="N35" t="n">
-        <v>387.732</v>
+        <v>88.51899999999999</v>
       </c>
       <c r="O35" t="n">
-        <v>567.285</v>
+        <v>1057.916</v>
       </c>
       <c r="P35" t="n">
-        <v>330.606</v>
+        <v>222.419</v>
       </c>
       <c r="Q35" t="n">
-        <v>24.514</v>
+        <v>24.528</v>
       </c>
       <c r="R35" t="n">
-        <v>21.223</v>
+        <v>22.774</v>
       </c>
       <c r="S35" t="n">
-        <v>18.817</v>
+        <v>28.084</v>
       </c>
       <c r="T35" t="n">
-        <v>9.917</v>
+        <v>4.168</v>
       </c>
       <c r="U35" t="n">
-        <v>27.799</v>
+        <v>27.565</v>
       </c>
       <c r="V35" t="n">
-        <v>227.731</v>
+        <v>52.83600000000001</v>
       </c>
       <c r="W35" t="n">
-        <v>344.608</v>
+        <v>446.2619999999999</v>
       </c>
       <c r="X35" t="n">
-        <v>144.429</v>
+        <v>160.213</v>
       </c>
     </row>
     <row r="36">
@@ -3140,74 +3140,74 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Voll- ein- Rudi- aus B</t>
+          <t>1/2 ein 1/2 aus B</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>38.72116666666667</v>
+        <v>29.174</v>
       </c>
       <c r="D36" t="n">
-        <v>39.17916666666667</v>
+        <v>29.073</v>
       </c>
       <c r="E36" t="n">
-        <v>-18.05266666666666</v>
+        <v>-9.818</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5445</v>
+        <v>3.523</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.996</v>
+        <v>1.067</v>
       </c>
       <c r="H36" t="n">
-        <v>-248.1423333333333</v>
+        <v>-126.883</v>
       </c>
       <c r="I36" t="n">
-        <v>-71.28583333333334</v>
+        <v>-49.182</v>
       </c>
       <c r="J36" t="n">
-        <v>-372.7196666666667</v>
+        <v>-150.656</v>
       </c>
       <c r="K36" t="n">
-        <v>-482.7015</v>
+        <v>-253.276</v>
       </c>
       <c r="L36" t="n">
-        <v>-139.3378333333334</v>
+        <v>-96.836</v>
       </c>
       <c r="M36" t="n">
-        <v>-727.5141666666667</v>
+        <v>-300.884</v>
       </c>
       <c r="N36" t="n">
-        <v>549.9928333333334</v>
+        <v>387.732</v>
       </c>
       <c r="O36" t="n">
-        <v>605.3473333333333</v>
+        <v>567.285</v>
       </c>
       <c r="P36" t="n">
-        <v>754.8053333333334</v>
+        <v>330.606</v>
       </c>
       <c r="Q36" t="n">
-        <v>22.0385</v>
+        <v>24.514</v>
       </c>
       <c r="R36" t="n">
-        <v>19.80833333333333</v>
+        <v>21.223</v>
       </c>
       <c r="S36" t="n">
-        <v>18.34916666666667</v>
+        <v>18.817</v>
       </c>
       <c r="T36" t="n">
-        <v>12.96533333333333</v>
+        <v>9.917</v>
       </c>
       <c r="U36" t="n">
-        <v>30.30566666666667</v>
+        <v>27.799</v>
       </c>
       <c r="V36" t="n">
-        <v>286.5363333333333</v>
+        <v>227.731</v>
       </c>
       <c r="W36" t="n">
-        <v>343.6168333333333</v>
+        <v>344.608</v>
       </c>
       <c r="X36" t="n">
-        <v>307.9193333333333</v>
+        <v>144.429</v>
       </c>
     </row>
     <row r="37">
@@ -3216,74 +3216,74 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus B</t>
+          <t>Voll- ein- Rudi- aus B</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>35.52258333333334</v>
+        <v>38.72116666666667</v>
       </c>
       <c r="D37" t="n">
-        <v>35.47925</v>
+        <v>39.17916666666667</v>
       </c>
       <c r="E37" t="n">
-        <v>-17.08525</v>
+        <v>-18.05266666666666</v>
       </c>
       <c r="F37" t="n">
-        <v>2.3225</v>
+        <v>0.5445</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.6322500000000001</v>
+        <v>-0.996</v>
       </c>
       <c r="H37" t="n">
-        <v>-204.9856666666667</v>
+        <v>-248.1423333333333</v>
       </c>
       <c r="I37" t="n">
-        <v>35.93783333333334</v>
+        <v>-71.28583333333334</v>
       </c>
       <c r="J37" t="n">
-        <v>-352.6988333333334</v>
+        <v>-372.7196666666667</v>
       </c>
       <c r="K37" t="n">
-        <v>-391.68625</v>
+        <v>-482.7015</v>
       </c>
       <c r="L37" t="n">
-        <v>70.16841666666666</v>
+        <v>-139.3378333333334</v>
       </c>
       <c r="M37" t="n">
-        <v>-675.18475</v>
+        <v>-727.5141666666667</v>
       </c>
       <c r="N37" t="n">
-        <v>467.4448333333333</v>
+        <v>549.9928333333334</v>
       </c>
       <c r="O37" t="n">
-        <v>573.3200000000001</v>
+        <v>605.3473333333333</v>
       </c>
       <c r="P37" t="n">
-        <v>700.6065</v>
+        <v>754.8053333333334</v>
       </c>
       <c r="Q37" t="n">
-        <v>22.26425</v>
+        <v>22.0385</v>
       </c>
       <c r="R37" t="n">
-        <v>18.84116666666666</v>
+        <v>19.80833333333333</v>
       </c>
       <c r="S37" t="n">
-        <v>20.24966666666667</v>
+        <v>18.34916666666667</v>
       </c>
       <c r="T37" t="n">
-        <v>9.648750000000001</v>
+        <v>12.96533333333333</v>
       </c>
       <c r="U37" t="n">
-        <v>28.16633333333334</v>
+        <v>30.30566666666667</v>
       </c>
       <c r="V37" t="n">
-        <v>248.3971666666667</v>
+        <v>286.5363333333333</v>
       </c>
       <c r="W37" t="n">
-        <v>333.7865</v>
+        <v>343.6168333333333</v>
       </c>
       <c r="X37" t="n">
-        <v>300.0774166666667</v>
+        <v>307.9193333333333</v>
       </c>
     </row>
     <row r="38">
@@ -3292,74 +3292,74 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Voll- ein- doppel- aus A</t>
+          <t>Voll- ein- voll- aus B</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>38.917</v>
+        <v>35.52258333333334</v>
       </c>
       <c r="D38" t="n">
-        <v>39.325</v>
+        <v>35.47925</v>
       </c>
       <c r="E38" t="n">
-        <v>-21.164</v>
+        <v>-17.08525</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.067</v>
+        <v>2.3225</v>
       </c>
       <c r="G38" t="n">
-        <v>-9.732999999999999</v>
+        <v>-0.6322500000000001</v>
       </c>
       <c r="H38" t="n">
-        <v>-234.922</v>
+        <v>-204.9856666666667</v>
       </c>
       <c r="I38" t="n">
-        <v>149.118</v>
+        <v>35.93783333333334</v>
       </c>
       <c r="J38" t="n">
-        <v>-423.3</v>
+        <v>-352.6988333333334</v>
       </c>
       <c r="K38" t="n">
-        <v>-386.035</v>
+        <v>-391.68625</v>
       </c>
       <c r="L38" t="n">
-        <v>246.065</v>
+        <v>70.16841666666666</v>
       </c>
       <c r="M38" t="n">
-        <v>-694.9960000000001</v>
+        <v>-675.18475</v>
       </c>
       <c r="N38" t="n">
-        <v>430.062</v>
+        <v>467.4448333333333</v>
       </c>
       <c r="O38" t="n">
-        <v>518.452</v>
+        <v>573.3200000000001</v>
       </c>
       <c r="P38" t="n">
-        <v>711.7860000000001</v>
+        <v>700.6065</v>
       </c>
       <c r="Q38" t="n">
-        <v>18.237</v>
+        <v>22.26425</v>
       </c>
       <c r="R38" t="n">
-        <v>15.672</v>
+        <v>18.84116666666666</v>
       </c>
       <c r="S38" t="n">
-        <v>18.538</v>
+        <v>20.24966666666667</v>
       </c>
       <c r="T38" t="n">
-        <v>6.112</v>
+        <v>9.648750000000001</v>
       </c>
       <c r="U38" t="n">
-        <v>27.456</v>
+        <v>28.16633333333334</v>
       </c>
       <c r="V38" t="n">
-        <v>247.65</v>
+        <v>248.3971666666667</v>
       </c>
       <c r="W38" t="n">
-        <v>300.818</v>
+        <v>333.7865</v>
       </c>
       <c r="X38" t="n">
-        <v>320.005</v>
+        <v>300.0774166666667</v>
       </c>
     </row>
     <row r="39">
@@ -3368,74 +3368,74 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Voll- ein- halb- aus B</t>
+          <t>Voll- ein- doppel- aus A</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>36.55214285714286</v>
+        <v>38.917</v>
       </c>
       <c r="D39" t="n">
-        <v>36.81114285714285</v>
+        <v>39.325</v>
       </c>
       <c r="E39" t="n">
-        <v>-17.67857142857143</v>
+        <v>-21.164</v>
       </c>
       <c r="F39" t="n">
-        <v>1.750285714285714</v>
+        <v>-0.067</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.837142857142857</v>
+        <v>-9.732999999999999</v>
       </c>
       <c r="H39" t="n">
-        <v>-166.2958571428572</v>
+        <v>-234.922</v>
       </c>
       <c r="I39" t="n">
-        <v>-148.081</v>
+        <v>149.118</v>
       </c>
       <c r="J39" t="n">
-        <v>-269.501</v>
+        <v>-423.3</v>
       </c>
       <c r="K39" t="n">
-        <v>-304.3057142857143</v>
+        <v>-386.035</v>
       </c>
       <c r="L39" t="n">
-        <v>-270.6174285714286</v>
+        <v>246.065</v>
       </c>
       <c r="M39" t="n">
-        <v>-491.251</v>
+        <v>-694.9960000000001</v>
       </c>
       <c r="N39" t="n">
-        <v>375.1785714285714</v>
+        <v>430.062</v>
       </c>
       <c r="O39" t="n">
-        <v>614.8082857142856</v>
+        <v>518.452</v>
       </c>
       <c r="P39" t="n">
-        <v>511.0224285714286</v>
+        <v>711.7860000000001</v>
       </c>
       <c r="Q39" t="n">
-        <v>21.43771428571429</v>
+        <v>18.237</v>
       </c>
       <c r="R39" t="n">
-        <v>19.43728571428571</v>
+        <v>15.672</v>
       </c>
       <c r="S39" t="n">
-        <v>18.40042857142857</v>
+        <v>18.538</v>
       </c>
       <c r="T39" t="n">
-        <v>10.96357142857143</v>
+        <v>6.112</v>
       </c>
       <c r="U39" t="n">
-        <v>29.04185714285714</v>
+        <v>27.456</v>
       </c>
       <c r="V39" t="n">
-        <v>241.8451428571429</v>
+        <v>247.65</v>
       </c>
       <c r="W39" t="n">
-        <v>363.649</v>
+        <v>300.818</v>
       </c>
       <c r="X39" t="n">
-        <v>261.0927142857143</v>
+        <v>320.005</v>
       </c>
     </row>
     <row r="40">
@@ -3444,74 +3444,74 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus A</t>
+          <t>Voll- ein- halb- aus B</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>37.57</v>
+        <v>36.55214285714286</v>
       </c>
       <c r="D40" t="n">
-        <v>37.72</v>
+        <v>36.81114285714285</v>
       </c>
       <c r="E40" t="n">
-        <v>-19.141</v>
+        <v>-17.67857142857143</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8183333333333334</v>
+        <v>1.750285714285714</v>
       </c>
       <c r="G40" t="n">
-        <v>-7.857333333333333</v>
+        <v>-1.837142857142857</v>
       </c>
       <c r="H40" t="n">
-        <v>-152.8063333333333</v>
+        <v>-166.2958571428572</v>
       </c>
       <c r="I40" t="n">
-        <v>148.8206666666667</v>
+        <v>-148.081</v>
       </c>
       <c r="J40" t="n">
-        <v>-394.2293333333334</v>
+        <v>-269.501</v>
       </c>
       <c r="K40" t="n">
-        <v>-265.355</v>
+        <v>-304.3057142857143</v>
       </c>
       <c r="L40" t="n">
-        <v>260.585</v>
+        <v>-270.6174285714286</v>
       </c>
       <c r="M40" t="n">
-        <v>-689.4616666666667</v>
+        <v>-491.251</v>
       </c>
       <c r="N40" t="n">
-        <v>376.7353333333333</v>
+        <v>375.1785714285714</v>
       </c>
       <c r="O40" t="n">
-        <v>524.3506666666667</v>
+        <v>614.8082857142856</v>
       </c>
       <c r="P40" t="n">
-        <v>720.4110000000001</v>
+        <v>511.0224285714286</v>
       </c>
       <c r="Q40" t="n">
-        <v>19.419</v>
+        <v>21.43771428571429</v>
       </c>
       <c r="R40" t="n">
-        <v>16.74333333333334</v>
+        <v>19.43728571428571</v>
       </c>
       <c r="S40" t="n">
-        <v>16.94133333333333</v>
+        <v>18.40042857142857</v>
       </c>
       <c r="T40" t="n">
-        <v>6.036333333333334</v>
+        <v>10.96357142857143</v>
       </c>
       <c r="U40" t="n">
-        <v>30.00833333333334</v>
+        <v>29.04185714285714</v>
       </c>
       <c r="V40" t="n">
-        <v>241.6536666666667</v>
+        <v>241.8451428571429</v>
       </c>
       <c r="W40" t="n">
-        <v>283.512</v>
+        <v>363.649</v>
       </c>
       <c r="X40" t="n">
-        <v>302.9816666666666</v>
+        <v>261.0927142857143</v>
       </c>
     </row>
     <row r="41">
@@ -3520,74 +3520,74 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Voll- ein- halb- aus C</t>
+          <t>Voll- ein- voll- aus A</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>35.57899999999999</v>
+        <v>37.57</v>
       </c>
       <c r="D41" t="n">
-        <v>36.006</v>
+        <v>37.72</v>
       </c>
       <c r="E41" t="n">
-        <v>-16.3615</v>
+        <v>-19.141</v>
       </c>
       <c r="F41" t="n">
-        <v>2.287</v>
+        <v>0.8183333333333334</v>
       </c>
       <c r="G41" t="n">
-        <v>-5.0425</v>
+        <v>-7.857333333333333</v>
       </c>
       <c r="H41" t="n">
-        <v>-193.664</v>
+        <v>-152.8063333333333</v>
       </c>
       <c r="I41" t="n">
-        <v>-106.441</v>
+        <v>148.8206666666667</v>
       </c>
       <c r="J41" t="n">
-        <v>-210.1095</v>
+        <v>-394.2293333333334</v>
       </c>
       <c r="K41" t="n">
-        <v>-361.5445</v>
+        <v>-265.355</v>
       </c>
       <c r="L41" t="n">
-        <v>-200.397</v>
+        <v>260.585</v>
       </c>
       <c r="M41" t="n">
-        <v>-390.9055</v>
+        <v>-689.4616666666667</v>
       </c>
       <c r="N41" t="n">
-        <v>429.688</v>
+        <v>376.7353333333333</v>
       </c>
       <c r="O41" t="n">
-        <v>589.9005</v>
+        <v>524.3506666666667</v>
       </c>
       <c r="P41" t="n">
-        <v>486.898</v>
+        <v>720.4110000000001</v>
       </c>
       <c r="Q41" t="n">
-        <v>23.2275</v>
+        <v>19.419</v>
       </c>
       <c r="R41" t="n">
-        <v>21.202</v>
+        <v>16.74333333333334</v>
       </c>
       <c r="S41" t="n">
-        <v>18.3185</v>
+        <v>16.94133333333333</v>
       </c>
       <c r="T41" t="n">
-        <v>8.118500000000001</v>
+        <v>6.036333333333334</v>
       </c>
       <c r="U41" t="n">
-        <v>30.281</v>
+        <v>30.00833333333334</v>
       </c>
       <c r="V41" t="n">
-        <v>271.813</v>
+        <v>241.6536666666667</v>
       </c>
       <c r="W41" t="n">
-        <v>340.7965</v>
+        <v>283.512</v>
       </c>
       <c r="X41" t="n">
-        <v>276.106</v>
+        <v>302.9816666666666</v>
       </c>
     </row>
     <row r="42">
@@ -3596,74 +3596,74 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus C</t>
+          <t>Voll- ein- halb- aus C</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>36.96</v>
+        <v>35.57899999999999</v>
       </c>
       <c r="D42" t="n">
-        <v>37.11533333333333</v>
+        <v>36.006</v>
       </c>
       <c r="E42" t="n">
-        <v>-19.18533333333333</v>
+        <v>-16.3615</v>
       </c>
       <c r="F42" t="n">
-        <v>1.532333333333333</v>
+        <v>2.287</v>
       </c>
       <c r="G42" t="n">
-        <v>-4.649</v>
+        <v>-5.0425</v>
       </c>
       <c r="H42" t="n">
-        <v>-234.7186666666666</v>
+        <v>-193.664</v>
       </c>
       <c r="I42" t="n">
-        <v>51.97133333333333</v>
+        <v>-106.441</v>
       </c>
       <c r="J42" t="n">
-        <v>-365.91</v>
+        <v>-210.1095</v>
       </c>
       <c r="K42" t="n">
-        <v>-412.3086666666666</v>
+        <v>-361.5445</v>
       </c>
       <c r="L42" t="n">
-        <v>96.87366666666667</v>
+        <v>-200.397</v>
       </c>
       <c r="M42" t="n">
-        <v>-644.6663333333335</v>
+        <v>-390.9055</v>
       </c>
       <c r="N42" t="n">
-        <v>434.0596666666667</v>
+        <v>429.688</v>
       </c>
       <c r="O42" t="n">
-        <v>522.3663333333334</v>
+        <v>589.9005</v>
       </c>
       <c r="P42" t="n">
-        <v>668.6133333333333</v>
+        <v>486.898</v>
       </c>
       <c r="Q42" t="n">
-        <v>19.804</v>
+        <v>23.2275</v>
       </c>
       <c r="R42" t="n">
-        <v>16.885</v>
+        <v>21.202</v>
       </c>
       <c r="S42" t="n">
-        <v>18.95833333333333</v>
+        <v>18.3185</v>
       </c>
       <c r="T42" t="n">
-        <v>6.530666666666666</v>
+        <v>8.118500000000001</v>
       </c>
       <c r="U42" t="n">
-        <v>28.20633333333333</v>
+        <v>30.281</v>
       </c>
       <c r="V42" t="n">
-        <v>231.889</v>
+        <v>271.813</v>
       </c>
       <c r="W42" t="n">
-        <v>315.9226666666667</v>
+        <v>340.7965</v>
       </c>
       <c r="X42" t="n">
-        <v>307.771</v>
+        <v>276.106</v>
       </c>
     </row>
     <row r="43">
@@ -3672,74 +3672,74 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Voll- ein 1 3/4 Salto vw C</t>
+          <t>Voll- ein- voll- aus C</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>29.22833333333334</v>
+        <v>36.96</v>
       </c>
       <c r="D43" t="n">
-        <v>29.149</v>
+        <v>37.11533333333333</v>
       </c>
       <c r="E43" t="n">
-        <v>-15.22433333333333</v>
+        <v>-19.18533333333333</v>
       </c>
       <c r="F43" t="n">
-        <v>-1.255</v>
+        <v>1.532333333333333</v>
       </c>
       <c r="G43" t="n">
-        <v>-1.538333333333333</v>
+        <v>-4.649</v>
       </c>
       <c r="H43" t="n">
-        <v>95.19566666666667</v>
+        <v>-234.7186666666666</v>
       </c>
       <c r="I43" t="n">
-        <v>-223.5676666666667</v>
+        <v>51.97133333333333</v>
       </c>
       <c r="J43" t="n">
-        <v>139.9815</v>
+        <v>-365.91</v>
       </c>
       <c r="K43" t="n">
-        <v>190.6551666666667</v>
+        <v>-412.3086666666666</v>
       </c>
       <c r="L43" t="n">
-        <v>-430.3043333333333</v>
+        <v>96.87366666666667</v>
       </c>
       <c r="M43" t="n">
-        <v>292.468</v>
+        <v>-644.6663333333335</v>
       </c>
       <c r="N43" t="n">
-        <v>348.5503333333334</v>
+        <v>434.0596666666667</v>
       </c>
       <c r="O43" t="n">
-        <v>505.584</v>
+        <v>522.3663333333334</v>
       </c>
       <c r="P43" t="n">
-        <v>333.5115</v>
+        <v>668.6133333333333</v>
       </c>
       <c r="Q43" t="n">
-        <v>23.06016666666666</v>
+        <v>19.804</v>
       </c>
       <c r="R43" t="n">
-        <v>19.757</v>
+        <v>16.885</v>
       </c>
       <c r="S43" t="n">
-        <v>15.19483333333333</v>
+        <v>18.95833333333333</v>
       </c>
       <c r="T43" t="n">
-        <v>7.741333333333333</v>
+        <v>6.530666666666666</v>
       </c>
       <c r="U43" t="n">
-        <v>24.45033333333333</v>
+        <v>28.20633333333333</v>
       </c>
       <c r="V43" t="n">
-        <v>230.0946666666667</v>
+        <v>231.889</v>
       </c>
       <c r="W43" t="n">
-        <v>193.8886666666667</v>
+        <v>315.9226666666667</v>
       </c>
       <c r="X43" t="n">
-        <v>200.9821666666667</v>
+        <v>307.771</v>
       </c>
     </row>
     <row r="44">
@@ -3748,74 +3748,74 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1 3/4 Salto vw C</t>
+          <t>Voll- ein 1 3/4 Salto vw C</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>26.8828</v>
+        <v>29.22833333333334</v>
       </c>
       <c r="D44" t="n">
-        <v>26.93</v>
+        <v>29.149</v>
       </c>
       <c r="E44" t="n">
-        <v>-14.5824</v>
+        <v>-15.22433333333333</v>
       </c>
       <c r="F44" t="n">
-        <v>0.0854</v>
+        <v>-1.255</v>
       </c>
       <c r="G44" t="n">
-        <v>0.9917999999999999</v>
+        <v>-1.538333333333333</v>
       </c>
       <c r="H44" t="n">
-        <v>6.622</v>
+        <v>95.19566666666667</v>
       </c>
       <c r="I44" t="n">
-        <v>-342.1744</v>
+        <v>-223.5676666666667</v>
       </c>
       <c r="J44" t="n">
-        <v>1.2608</v>
+        <v>139.9815</v>
       </c>
       <c r="K44" t="n">
-        <v>17.9002</v>
+        <v>190.6551666666667</v>
       </c>
       <c r="L44" t="n">
-        <v>-661.8158000000001</v>
+        <v>-430.3043333333333</v>
       </c>
       <c r="M44" t="n">
-        <v>24.689</v>
+        <v>292.468</v>
       </c>
       <c r="N44" t="n">
-        <v>38.9594</v>
+        <v>348.5503333333334</v>
       </c>
       <c r="O44" t="n">
-        <v>673.4341999999999</v>
+        <v>505.584</v>
       </c>
       <c r="P44" t="n">
-        <v>60.08000000000001</v>
+        <v>333.5115</v>
       </c>
       <c r="Q44" t="n">
-        <v>25.9652</v>
+        <v>23.06016666666666</v>
       </c>
       <c r="R44" t="n">
-        <v>22.9034</v>
+        <v>19.757</v>
       </c>
       <c r="S44" t="n">
-        <v>18.4732</v>
+        <v>15.19483333333333</v>
       </c>
       <c r="T44" t="n">
-        <v>1.9258</v>
+        <v>7.741333333333333</v>
       </c>
       <c r="U44" t="n">
-        <v>24.0882</v>
+        <v>24.45033333333333</v>
       </c>
       <c r="V44" t="n">
-        <v>19.041</v>
+        <v>230.0946666666667</v>
       </c>
       <c r="W44" t="n">
-        <v>200.656</v>
+        <v>193.8886666666667</v>
       </c>
       <c r="X44" t="n">
-        <v>26.8358</v>
+        <v>200.9821666666667</v>
       </c>
     </row>
     <row r="45">
@@ -3824,74 +3824,74 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Triffis B</t>
+          <t>1 3/4 Salto vw C</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>45.343</v>
+        <v>26.8828</v>
       </c>
       <c r="D45" t="n">
-        <v>45.5032</v>
+        <v>26.93</v>
       </c>
       <c r="E45" t="n">
-        <v>-27.2924</v>
+        <v>-14.5824</v>
       </c>
       <c r="F45" t="n">
-        <v>6.956999999999999</v>
+        <v>0.0854</v>
       </c>
       <c r="G45" t="n">
-        <v>-2.6092</v>
+        <v>0.9917999999999999</v>
       </c>
       <c r="H45" t="n">
-        <v>-98.2574</v>
+        <v>6.622</v>
       </c>
       <c r="I45" t="n">
-        <v>-368.478</v>
+        <v>-342.1744</v>
       </c>
       <c r="J45" t="n">
-        <v>-94.74039999999999</v>
+        <v>1.2608</v>
       </c>
       <c r="K45" t="n">
-        <v>-195.0148</v>
+        <v>17.9002</v>
       </c>
       <c r="L45" t="n">
-        <v>-732.9498000000001</v>
+        <v>-661.8158000000001</v>
       </c>
       <c r="M45" t="n">
-        <v>-188.6016</v>
+        <v>24.689</v>
       </c>
       <c r="N45" t="n">
-        <v>316.7212000000001</v>
+        <v>38.9594</v>
       </c>
       <c r="O45" t="n">
-        <v>982.6779999999999</v>
+        <v>673.4341999999999</v>
       </c>
       <c r="P45" t="n">
-        <v>278.2516</v>
+        <v>60.08000000000001</v>
       </c>
       <c r="Q45" t="n">
-        <v>23.2562</v>
+        <v>25.9652</v>
       </c>
       <c r="R45" t="n">
-        <v>21.3198</v>
+        <v>22.9034</v>
       </c>
       <c r="S45" t="n">
-        <v>24.5062</v>
+        <v>18.4732</v>
       </c>
       <c r="T45" t="n">
-        <v>9.521800000000001</v>
+        <v>1.9258</v>
       </c>
       <c r="U45" t="n">
-        <v>30.622</v>
+        <v>24.0882</v>
       </c>
       <c r="V45" t="n">
-        <v>163.7492</v>
+        <v>19.041</v>
       </c>
       <c r="W45" t="n">
-        <v>431.4264</v>
+        <v>200.656</v>
       </c>
       <c r="X45" t="n">
-        <v>173.0902</v>
+        <v>26.8358</v>
       </c>
     </row>
     <row r="46">
@@ -3900,74 +3900,74 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Halb- ein- halb- aus B</t>
+          <t>Triffis B</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>35.128</v>
+        <v>45.343</v>
       </c>
       <c r="D46" t="n">
-        <v>34.865</v>
+        <v>45.5032</v>
       </c>
       <c r="E46" t="n">
-        <v>-16.819</v>
+        <v>-27.2924</v>
       </c>
       <c r="F46" t="n">
-        <v>4.405</v>
+        <v>6.956999999999999</v>
       </c>
       <c r="G46" t="n">
-        <v>-2.158</v>
+        <v>-2.6092</v>
       </c>
       <c r="H46" t="n">
-        <v>-125.656</v>
+        <v>-98.2574</v>
       </c>
       <c r="I46" t="n">
-        <v>-85.64200000000001</v>
+        <v>-368.478</v>
       </c>
       <c r="J46" t="n">
-        <v>-167.185</v>
+        <v>-94.74039999999999</v>
       </c>
       <c r="K46" t="n">
-        <v>-215.313</v>
+        <v>-195.0148</v>
       </c>
       <c r="L46" t="n">
-        <v>-143.538</v>
+        <v>-732.9498000000001</v>
       </c>
       <c r="M46" t="n">
-        <v>-286.615</v>
+        <v>-188.6016</v>
       </c>
       <c r="N46" t="n">
-        <v>322.824</v>
+        <v>316.7212000000001</v>
       </c>
       <c r="O46" t="n">
-        <v>575.2809999999999</v>
+        <v>982.6779999999999</v>
       </c>
       <c r="P46" t="n">
-        <v>370.702</v>
+        <v>278.2516</v>
       </c>
       <c r="Q46" t="n">
-        <v>21.684</v>
+        <v>23.2562</v>
       </c>
       <c r="R46" t="n">
-        <v>18.348</v>
+        <v>21.3198</v>
       </c>
       <c r="S46" t="n">
-        <v>18.576</v>
+        <v>24.5062</v>
       </c>
       <c r="T46" t="n">
-        <v>9.635</v>
+        <v>9.521800000000001</v>
       </c>
       <c r="U46" t="n">
-        <v>28.464</v>
+        <v>30.622</v>
       </c>
       <c r="V46" t="n">
-        <v>210.182</v>
+        <v>163.7492</v>
       </c>
       <c r="W46" t="n">
-        <v>379.163</v>
+        <v>431.4264</v>
       </c>
       <c r="X46" t="n">
-        <v>200.306</v>
+        <v>173.0902</v>
       </c>
     </row>
     <row r="47">
@@ -3976,74 +3976,74 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Halb- ein- halb- aus C</t>
+          <t>Halb- ein- halb- aus B</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>36.678</v>
+        <v>35.128</v>
       </c>
       <c r="D47" t="n">
-        <v>36.472</v>
+        <v>34.865</v>
       </c>
       <c r="E47" t="n">
-        <v>-17.34</v>
+        <v>-16.819</v>
       </c>
       <c r="F47" t="n">
-        <v>3.319</v>
+        <v>4.405</v>
       </c>
       <c r="G47" t="n">
-        <v>-4.671</v>
+        <v>-2.158</v>
       </c>
       <c r="H47" t="n">
-        <v>-120.127</v>
+        <v>-125.656</v>
       </c>
       <c r="I47" t="n">
-        <v>-97.44</v>
+        <v>-85.64200000000001</v>
       </c>
       <c r="J47" t="n">
-        <v>-155.547</v>
+        <v>-167.185</v>
       </c>
       <c r="K47" t="n">
-        <v>-205.367</v>
+        <v>-215.313</v>
       </c>
       <c r="L47" t="n">
-        <v>-165.06</v>
+        <v>-143.538</v>
       </c>
       <c r="M47" t="n">
-        <v>-265.518</v>
+        <v>-286.615</v>
       </c>
       <c r="N47" t="n">
-        <v>297.207</v>
+        <v>322.824</v>
       </c>
       <c r="O47" t="n">
-        <v>584.437</v>
+        <v>575.2809999999999</v>
       </c>
       <c r="P47" t="n">
-        <v>366.502</v>
+        <v>370.702</v>
       </c>
       <c r="Q47" t="n">
-        <v>23.556</v>
+        <v>21.684</v>
       </c>
       <c r="R47" t="n">
-        <v>20.994</v>
+        <v>18.348</v>
       </c>
       <c r="S47" t="n">
-        <v>22.72</v>
+        <v>18.576</v>
       </c>
       <c r="T47" t="n">
-        <v>8.277999999999999</v>
+        <v>9.635</v>
       </c>
       <c r="U47" t="n">
-        <v>28.907</v>
+        <v>28.464</v>
       </c>
       <c r="V47" t="n">
-        <v>208.485</v>
+        <v>210.182</v>
       </c>
       <c r="W47" t="n">
-        <v>393.7380000000001</v>
+        <v>379.163</v>
       </c>
       <c r="X47" t="n">
-        <v>199.733</v>
+        <v>200.306</v>
       </c>
     </row>
     <row r="48">
@@ -4052,74 +4052,74 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Halb- ein- Rudy- aus B</t>
+          <t>Halb- ein- halb- aus C</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>39.131</v>
+        <v>36.678</v>
       </c>
       <c r="D48" t="n">
-        <v>39.188</v>
+        <v>36.472</v>
       </c>
       <c r="E48" t="n">
-        <v>-19.987</v>
+        <v>-17.34</v>
       </c>
       <c r="F48" t="n">
-        <v>2.927</v>
+        <v>3.319</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.328</v>
+        <v>-4.671</v>
       </c>
       <c r="H48" t="n">
-        <v>-195.663</v>
+        <v>-120.127</v>
       </c>
       <c r="I48" t="n">
-        <v>-3.235</v>
+        <v>-97.44</v>
       </c>
       <c r="J48" t="n">
-        <v>-361.304</v>
+        <v>-155.547</v>
       </c>
       <c r="K48" t="n">
-        <v>-368.043</v>
+        <v>-205.367</v>
       </c>
       <c r="L48" t="n">
-        <v>-4.551</v>
+        <v>-165.06</v>
       </c>
       <c r="M48" t="n">
-        <v>-680.7089999999999</v>
+        <v>-265.518</v>
       </c>
       <c r="N48" t="n">
-        <v>477.2430000000001</v>
+        <v>297.207</v>
       </c>
       <c r="O48" t="n">
-        <v>571.381</v>
+        <v>584.437</v>
       </c>
       <c r="P48" t="n">
-        <v>696.701</v>
+        <v>366.502</v>
       </c>
       <c r="Q48" t="n">
-        <v>22.256</v>
+        <v>23.556</v>
       </c>
       <c r="R48" t="n">
-        <v>18.544</v>
+        <v>20.994</v>
       </c>
       <c r="S48" t="n">
-        <v>19.263</v>
+        <v>22.72</v>
       </c>
       <c r="T48" t="n">
-        <v>13.373</v>
+        <v>8.277999999999999</v>
       </c>
       <c r="U48" t="n">
-        <v>29.654</v>
+        <v>28.907</v>
       </c>
       <c r="V48" t="n">
-        <v>247.62</v>
+        <v>208.485</v>
       </c>
       <c r="W48" t="n">
-        <v>354.3</v>
+        <v>393.7380000000001</v>
       </c>
       <c r="X48" t="n">
-        <v>291.56</v>
+        <v>199.733</v>
       </c>
     </row>
     <row r="49">
@@ -4128,74 +4128,74 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Schraubensalto C</t>
+          <t>Halb- ein- Rudy- aus B</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>17.13769387755102</v>
+        <v>39.131</v>
       </c>
       <c r="D49" t="n">
-        <v>17.03928571428571</v>
+        <v>39.188</v>
       </c>
       <c r="E49" t="n">
-        <v>-2.480428571428572</v>
+        <v>-19.987</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.7355306122448979</v>
+        <v>2.927</v>
       </c>
       <c r="G49" t="n">
-        <v>5.578591836734695</v>
+        <v>-1.328</v>
       </c>
       <c r="H49" t="n">
-        <v>41.7034693877551</v>
+        <v>-195.663</v>
       </c>
       <c r="I49" t="n">
-        <v>93.78261224489798</v>
+        <v>-3.235</v>
       </c>
       <c r="J49" t="n">
-        <v>211.2369591836735</v>
+        <v>-361.304</v>
       </c>
       <c r="K49" t="n">
-        <v>78.98699999999999</v>
+        <v>-368.043</v>
       </c>
       <c r="L49" t="n">
-        <v>175.5836938775511</v>
+        <v>-4.551</v>
       </c>
       <c r="M49" t="n">
-        <v>395.8561224489796</v>
+        <v>-680.7089999999999</v>
       </c>
       <c r="N49" t="n">
-        <v>162.7044489795918</v>
+        <v>477.2430000000001</v>
       </c>
       <c r="O49" t="n">
-        <v>280.2916122448979</v>
+        <v>571.381</v>
       </c>
       <c r="P49" t="n">
-        <v>400.5705918367346</v>
+        <v>696.701</v>
       </c>
       <c r="Q49" t="n">
-        <v>23.09702040816326</v>
+        <v>22.256</v>
       </c>
       <c r="R49" t="n">
-        <v>20.62551020408163</v>
+        <v>18.544</v>
       </c>
       <c r="S49" t="n">
-        <v>10.63020408163265</v>
+        <v>19.263</v>
       </c>
       <c r="T49" t="n">
-        <v>2.629204081632653</v>
+        <v>13.373</v>
       </c>
       <c r="U49" t="n">
-        <v>24.45461224489796</v>
+        <v>29.654</v>
       </c>
       <c r="V49" t="n">
-        <v>106.5022244897959</v>
+        <v>247.62</v>
       </c>
       <c r="W49" t="n">
-        <v>129.5556326530612</v>
+        <v>354.3</v>
       </c>
       <c r="X49" t="n">
-        <v>162.0674693877551</v>
+        <v>291.56</v>
       </c>
     </row>
     <row r="50">
@@ -4204,74 +4204,74 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Bauchsprung</t>
+          <t>Schraubensalto C</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>11.95702702702703</v>
+        <v>17.13769387755102</v>
       </c>
       <c r="D50" t="n">
-        <v>11.32617567567567</v>
+        <v>17.03928571428571</v>
       </c>
       <c r="E50" t="n">
-        <v>4.756094594594595</v>
+        <v>-2.480428571428572</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.1839594594594595</v>
+        <v>-0.7355306122448979</v>
       </c>
       <c r="G50" t="n">
-        <v>7.233013513513512</v>
+        <v>5.578591836734695</v>
       </c>
       <c r="H50" t="n">
-        <v>-2.007094594594595</v>
+        <v>41.7034693877551</v>
       </c>
       <c r="I50" t="n">
-        <v>-21.71147297297297</v>
+        <v>93.78261224489798</v>
       </c>
       <c r="J50" t="n">
-        <v>-4.42981081081081</v>
+        <v>211.2369591836735</v>
       </c>
       <c r="K50" t="n">
-        <v>-3.847472972972974</v>
+        <v>78.98699999999999</v>
       </c>
       <c r="L50" t="n">
-        <v>-38.9775</v>
+        <v>175.5836938775511</v>
       </c>
       <c r="M50" t="n">
-        <v>-8.317594594594594</v>
+        <v>395.8561224489796</v>
       </c>
       <c r="N50" t="n">
-        <v>21.71535135135135</v>
+        <v>162.7044489795918</v>
       </c>
       <c r="O50" t="n">
-        <v>119.7072567567568</v>
+        <v>280.2916122448979</v>
       </c>
       <c r="P50" t="n">
-        <v>35.68600000000001</v>
+        <v>400.5705918367346</v>
       </c>
       <c r="Q50" t="n">
-        <v>24.26571621621622</v>
+        <v>23.09702040816326</v>
       </c>
       <c r="R50" t="n">
-        <v>21.49163513513514</v>
+        <v>20.62551020408163</v>
       </c>
       <c r="S50" t="n">
-        <v>15.04294594594595</v>
+        <v>10.63020408163265</v>
       </c>
       <c r="T50" t="n">
-        <v>1.200878378378379</v>
+        <v>2.629204081632653</v>
       </c>
       <c r="U50" t="n">
-        <v>19.41366216216217</v>
+        <v>24.45461224489796</v>
       </c>
       <c r="V50" t="n">
-        <v>12.90618918918919</v>
+        <v>106.5022244897959</v>
       </c>
       <c r="W50" t="n">
-        <v>71.9982972972973</v>
+        <v>129.5556326530612</v>
       </c>
       <c r="X50" t="n">
-        <v>19.88351351351351</v>
+        <v>162.0674693877551</v>
       </c>
     </row>
     <row r="51">
@@ -4280,73 +4280,149 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Bauchsprung</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>11.95702702702703</v>
+      </c>
+      <c r="D51" t="n">
+        <v>11.32617567567567</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4.756094594594595</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-0.1839594594594595</v>
+      </c>
+      <c r="G51" t="n">
+        <v>7.233013513513512</v>
+      </c>
+      <c r="H51" t="n">
+        <v>-2.007094594594595</v>
+      </c>
+      <c r="I51" t="n">
+        <v>-21.71147297297297</v>
+      </c>
+      <c r="J51" t="n">
+        <v>-4.42981081081081</v>
+      </c>
+      <c r="K51" t="n">
+        <v>-3.847472972972974</v>
+      </c>
+      <c r="L51" t="n">
+        <v>-38.9775</v>
+      </c>
+      <c r="M51" t="n">
+        <v>-8.317594594594594</v>
+      </c>
+      <c r="N51" t="n">
+        <v>21.71535135135135</v>
+      </c>
+      <c r="O51" t="n">
+        <v>119.7072567567568</v>
+      </c>
+      <c r="P51" t="n">
+        <v>35.68600000000001</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>24.26571621621622</v>
+      </c>
+      <c r="R51" t="n">
+        <v>21.49163513513514</v>
+      </c>
+      <c r="S51" t="n">
+        <v>15.04294594594595</v>
+      </c>
+      <c r="T51" t="n">
+        <v>1.200878378378379</v>
+      </c>
+      <c r="U51" t="n">
+        <v>19.41366216216217</v>
+      </c>
+      <c r="V51" t="n">
+        <v>12.90618918918919</v>
+      </c>
+      <c r="W51" t="n">
+        <v>71.9982972972973</v>
+      </c>
+      <c r="X51" t="n">
+        <v>19.88351351351351</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>Von Bauch in Stand</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="C52" t="n">
         <v>12.73906756756757</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>13.21222972972973</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E52" t="n">
         <v>6.384635135135134</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F52" t="n">
         <v>-0.01454054054054054</v>
       </c>
-      <c r="G51" t="n">
+      <c r="G52" t="n">
         <v>6.474905405405406</v>
       </c>
-      <c r="H51" t="n">
+      <c r="H52" t="n">
         <v>2.209797297297297</v>
       </c>
-      <c r="I51" t="n">
+      <c r="I52" t="n">
         <v>22.75035135135135</v>
       </c>
-      <c r="J51" t="n">
+      <c r="J52" t="n">
         <v>3.928756756756756</v>
       </c>
-      <c r="K51" t="n">
+      <c r="K52" t="n">
         <v>3.957702702702702</v>
       </c>
-      <c r="L51" t="n">
+      <c r="L52" t="n">
         <v>38.25474324324325</v>
       </c>
-      <c r="M51" t="n">
+      <c r="M52" t="n">
         <v>7.01945945945946</v>
       </c>
-      <c r="N51" t="n">
+      <c r="N52" t="n">
         <v>25.20467567567567</v>
       </c>
-      <c r="O51" t="n">
+      <c r="O52" t="n">
         <v>83.52685135135135</v>
       </c>
-      <c r="P51" t="n">
+      <c r="P52" t="n">
         <v>40.98166216216216</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="Q52" t="n">
         <v>24.26547297297298</v>
       </c>
-      <c r="R51" t="n">
+      <c r="R52" t="n">
         <v>24.46771621621621</v>
       </c>
-      <c r="S51" t="n">
+      <c r="S52" t="n">
         <v>16.66471621621622</v>
       </c>
-      <c r="T51" t="n">
+      <c r="T52" t="n">
         <v>1.57622972972973</v>
       </c>
-      <c r="U51" t="n">
+      <c r="U52" t="n">
         <v>17.78168918918919</v>
       </c>
-      <c r="V51" t="n">
+      <c r="V52" t="n">
         <v>15.6312027027027</v>
       </c>
-      <c r="W51" t="n">
+      <c r="W52" t="n">
         <v>64.54325675675676</v>
       </c>
-      <c r="X51" t="n">
+      <c r="X52" t="n">
         <v>21.76814864864865</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another spelling error correction
</commit_message>
<xml_diff>
--- a/Sprungdaten_processed/class_std_mean.xlsx
+++ b/Sprungdaten_processed/class_std_mean.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2308,70 +2308,70 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>14.811</v>
+        <v>14.85416666666667</v>
       </c>
       <c r="D25" t="n">
-        <v>14.7015</v>
+        <v>14.68638888888889</v>
       </c>
       <c r="E25" t="n">
-        <v>-1.875375</v>
+        <v>-3.885555555555556</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.6473749999999999</v>
+        <v>-0.5276111111111111</v>
       </c>
       <c r="G25" t="n">
-        <v>5.05025</v>
+        <v>4.780166666666667</v>
       </c>
       <c r="H25" t="n">
-        <v>8.1205</v>
+        <v>4.871722222222222</v>
       </c>
       <c r="I25" t="n">
-        <v>-36.26512499999999</v>
+        <v>-103.4526111111111</v>
       </c>
       <c r="J25" t="n">
-        <v>13.29325</v>
+        <v>11.48588888888889</v>
       </c>
       <c r="K25" t="n">
-        <v>13.04425</v>
+        <v>8.303666666666667</v>
       </c>
       <c r="L25" t="n">
-        <v>-66.11762499999999</v>
+        <v>-183.2552222222222</v>
       </c>
       <c r="M25" t="n">
-        <v>20.946125</v>
+        <v>17.70605555555555</v>
       </c>
       <c r="N25" t="n">
-        <v>34.19675</v>
+        <v>27.54405555555556</v>
       </c>
       <c r="O25" t="n">
-        <v>304.482625</v>
+        <v>304.8005</v>
       </c>
       <c r="P25" t="n">
-        <v>53.268125</v>
+        <v>46.03177777777778</v>
       </c>
       <c r="Q25" t="n">
-        <v>27.243875</v>
+        <v>27.64738888888889</v>
       </c>
       <c r="R25" t="n">
-        <v>23.109625</v>
+        <v>23.23311111111111</v>
       </c>
       <c r="S25" t="n">
-        <v>16.093875</v>
+        <v>16.90227777777778</v>
       </c>
       <c r="T25" t="n">
-        <v>1.971625</v>
+        <v>1.644611111111111</v>
       </c>
       <c r="U25" t="n">
-        <v>20.625375</v>
+        <v>20.24066666666666</v>
       </c>
       <c r="V25" t="n">
-        <v>13.86125</v>
+        <v>12.91516666666667</v>
       </c>
       <c r="W25" t="n">
-        <v>123.710125</v>
+        <v>122.5273888888889</v>
       </c>
       <c r="X25" t="n">
-        <v>23.838875</v>
+        <v>20.08138888888889</v>
       </c>
     </row>
     <row r="26">
@@ -2988,74 +2988,74 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/4 Salto Vw A</t>
+          <t>Triffis C</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>14.8887</v>
+        <v>45.26</v>
       </c>
       <c r="D34" t="n">
-        <v>14.6743</v>
+        <v>45.75</v>
       </c>
       <c r="E34" t="n">
-        <v>-5.4937</v>
+        <v>-29.881</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.4318</v>
+        <v>-0.619</v>
       </c>
       <c r="G34" t="n">
-        <v>4.5641</v>
+        <v>3.723</v>
       </c>
       <c r="H34" t="n">
-        <v>2.2727</v>
+        <v>-18.669</v>
       </c>
       <c r="I34" t="n">
-        <v>-157.2026</v>
+        <v>-395.789</v>
       </c>
       <c r="J34" t="n">
-        <v>10.04</v>
+        <v>-82.48999999999999</v>
       </c>
       <c r="K34" t="n">
-        <v>4.5112</v>
+        <v>-37.545</v>
       </c>
       <c r="L34" t="n">
-        <v>-276.9653</v>
+        <v>-804.385</v>
       </c>
       <c r="M34" t="n">
-        <v>15.114</v>
+        <v>-167.241</v>
       </c>
       <c r="N34" t="n">
-        <v>22.2219</v>
+        <v>88.51899999999999</v>
       </c>
       <c r="O34" t="n">
-        <v>305.0548</v>
+        <v>1057.916</v>
       </c>
       <c r="P34" t="n">
-        <v>40.2427</v>
+        <v>222.419</v>
       </c>
       <c r="Q34" t="n">
-        <v>27.9702</v>
+        <v>24.528</v>
       </c>
       <c r="R34" t="n">
-        <v>23.3319</v>
+        <v>22.774</v>
       </c>
       <c r="S34" t="n">
-        <v>17.549</v>
+        <v>28.084</v>
       </c>
       <c r="T34" t="n">
-        <v>1.383</v>
+        <v>4.168</v>
       </c>
       <c r="U34" t="n">
-        <v>19.9329</v>
+        <v>27.565</v>
       </c>
       <c r="V34" t="n">
-        <v>12.1583</v>
+        <v>52.83600000000001</v>
       </c>
       <c r="W34" t="n">
-        <v>121.5812</v>
+        <v>446.2619999999999</v>
       </c>
       <c r="X34" t="n">
-        <v>17.0754</v>
+        <v>160.213</v>
       </c>
     </row>
     <row r="35">
@@ -3064,74 +3064,74 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Triffis C</t>
+          <t>1/2 ein 1/2 aus B</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>45.26</v>
+        <v>29.174</v>
       </c>
       <c r="D35" t="n">
-        <v>45.75</v>
+        <v>29.073</v>
       </c>
       <c r="E35" t="n">
-        <v>-29.881</v>
+        <v>-9.818</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.619</v>
+        <v>3.523</v>
       </c>
       <c r="G35" t="n">
-        <v>3.723</v>
+        <v>1.067</v>
       </c>
       <c r="H35" t="n">
-        <v>-18.669</v>
+        <v>-126.883</v>
       </c>
       <c r="I35" t="n">
-        <v>-395.789</v>
+        <v>-49.182</v>
       </c>
       <c r="J35" t="n">
-        <v>-82.48999999999999</v>
+        <v>-150.656</v>
       </c>
       <c r="K35" t="n">
-        <v>-37.545</v>
+        <v>-253.276</v>
       </c>
       <c r="L35" t="n">
-        <v>-804.385</v>
+        <v>-96.836</v>
       </c>
       <c r="M35" t="n">
-        <v>-167.241</v>
+        <v>-300.884</v>
       </c>
       <c r="N35" t="n">
-        <v>88.51899999999999</v>
+        <v>387.732</v>
       </c>
       <c r="O35" t="n">
-        <v>1057.916</v>
+        <v>567.285</v>
       </c>
       <c r="P35" t="n">
-        <v>222.419</v>
+        <v>330.606</v>
       </c>
       <c r="Q35" t="n">
-        <v>24.528</v>
+        <v>24.514</v>
       </c>
       <c r="R35" t="n">
-        <v>22.774</v>
+        <v>21.223</v>
       </c>
       <c r="S35" t="n">
-        <v>28.084</v>
+        <v>18.817</v>
       </c>
       <c r="T35" t="n">
-        <v>4.168</v>
+        <v>9.917</v>
       </c>
       <c r="U35" t="n">
-        <v>27.565</v>
+        <v>27.799</v>
       </c>
       <c r="V35" t="n">
-        <v>52.83600000000001</v>
+        <v>227.731</v>
       </c>
       <c r="W35" t="n">
-        <v>446.2619999999999</v>
+        <v>344.608</v>
       </c>
       <c r="X35" t="n">
-        <v>160.213</v>
+        <v>144.429</v>
       </c>
     </row>
     <row r="36">
@@ -3140,74 +3140,74 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1/2 ein 1/2 aus B</t>
+          <t>Voll- ein- Rudi- aus B</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>29.174</v>
+        <v>38.72116666666667</v>
       </c>
       <c r="D36" t="n">
-        <v>29.073</v>
+        <v>39.17916666666667</v>
       </c>
       <c r="E36" t="n">
-        <v>-9.818</v>
+        <v>-18.05266666666666</v>
       </c>
       <c r="F36" t="n">
-        <v>3.523</v>
+        <v>0.5445</v>
       </c>
       <c r="G36" t="n">
-        <v>1.067</v>
+        <v>-0.996</v>
       </c>
       <c r="H36" t="n">
-        <v>-126.883</v>
+        <v>-248.1423333333333</v>
       </c>
       <c r="I36" t="n">
-        <v>-49.182</v>
+        <v>-71.28583333333334</v>
       </c>
       <c r="J36" t="n">
-        <v>-150.656</v>
+        <v>-372.7196666666667</v>
       </c>
       <c r="K36" t="n">
-        <v>-253.276</v>
+        <v>-482.7015</v>
       </c>
       <c r="L36" t="n">
-        <v>-96.836</v>
+        <v>-139.3378333333334</v>
       </c>
       <c r="M36" t="n">
-        <v>-300.884</v>
+        <v>-727.5141666666667</v>
       </c>
       <c r="N36" t="n">
-        <v>387.732</v>
+        <v>549.9928333333334</v>
       </c>
       <c r="O36" t="n">
-        <v>567.285</v>
+        <v>605.3473333333333</v>
       </c>
       <c r="P36" t="n">
-        <v>330.606</v>
+        <v>754.8053333333334</v>
       </c>
       <c r="Q36" t="n">
-        <v>24.514</v>
+        <v>22.0385</v>
       </c>
       <c r="R36" t="n">
-        <v>21.223</v>
+        <v>19.80833333333333</v>
       </c>
       <c r="S36" t="n">
-        <v>18.817</v>
+        <v>18.34916666666667</v>
       </c>
       <c r="T36" t="n">
-        <v>9.917</v>
+        <v>12.96533333333333</v>
       </c>
       <c r="U36" t="n">
-        <v>27.799</v>
+        <v>30.30566666666667</v>
       </c>
       <c r="V36" t="n">
-        <v>227.731</v>
+        <v>286.5363333333333</v>
       </c>
       <c r="W36" t="n">
-        <v>344.608</v>
+        <v>343.6168333333333</v>
       </c>
       <c r="X36" t="n">
-        <v>144.429</v>
+        <v>307.9193333333333</v>
       </c>
     </row>
     <row r="37">
@@ -3216,74 +3216,74 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Voll- ein- Rudi- aus B</t>
+          <t>Voll- ein- voll- aus B</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>38.72116666666667</v>
+        <v>35.52258333333334</v>
       </c>
       <c r="D37" t="n">
-        <v>39.17916666666667</v>
+        <v>35.47925</v>
       </c>
       <c r="E37" t="n">
-        <v>-18.05266666666666</v>
+        <v>-17.08525</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5445</v>
+        <v>2.3225</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.996</v>
+        <v>-0.6322500000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>-248.1423333333333</v>
+        <v>-204.9856666666667</v>
       </c>
       <c r="I37" t="n">
-        <v>-71.28583333333334</v>
+        <v>35.93783333333334</v>
       </c>
       <c r="J37" t="n">
-        <v>-372.7196666666667</v>
+        <v>-352.6988333333334</v>
       </c>
       <c r="K37" t="n">
-        <v>-482.7015</v>
+        <v>-391.68625</v>
       </c>
       <c r="L37" t="n">
-        <v>-139.3378333333334</v>
+        <v>70.16841666666666</v>
       </c>
       <c r="M37" t="n">
-        <v>-727.5141666666667</v>
+        <v>-675.18475</v>
       </c>
       <c r="N37" t="n">
-        <v>549.9928333333334</v>
+        <v>467.4448333333333</v>
       </c>
       <c r="O37" t="n">
-        <v>605.3473333333333</v>
+        <v>573.3200000000001</v>
       </c>
       <c r="P37" t="n">
-        <v>754.8053333333334</v>
+        <v>700.6065</v>
       </c>
       <c r="Q37" t="n">
-        <v>22.0385</v>
+        <v>22.26425</v>
       </c>
       <c r="R37" t="n">
-        <v>19.80833333333333</v>
+        <v>18.84116666666666</v>
       </c>
       <c r="S37" t="n">
-        <v>18.34916666666667</v>
+        <v>20.24966666666667</v>
       </c>
       <c r="T37" t="n">
-        <v>12.96533333333333</v>
+        <v>9.648750000000001</v>
       </c>
       <c r="U37" t="n">
-        <v>30.30566666666667</v>
+        <v>28.16633333333334</v>
       </c>
       <c r="V37" t="n">
-        <v>286.5363333333333</v>
+        <v>248.3971666666667</v>
       </c>
       <c r="W37" t="n">
-        <v>343.6168333333333</v>
+        <v>333.7865</v>
       </c>
       <c r="X37" t="n">
-        <v>307.9193333333333</v>
+        <v>300.0774166666667</v>
       </c>
     </row>
     <row r="38">
@@ -3292,74 +3292,74 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus B</t>
+          <t>Voll- ein- doppel- aus A</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>35.52258333333334</v>
+        <v>38.917</v>
       </c>
       <c r="D38" t="n">
-        <v>35.47925</v>
+        <v>39.325</v>
       </c>
       <c r="E38" t="n">
-        <v>-17.08525</v>
+        <v>-21.164</v>
       </c>
       <c r="F38" t="n">
-        <v>2.3225</v>
+        <v>-0.067</v>
       </c>
       <c r="G38" t="n">
-        <v>-0.6322500000000001</v>
+        <v>-9.732999999999999</v>
       </c>
       <c r="H38" t="n">
-        <v>-204.9856666666667</v>
+        <v>-234.922</v>
       </c>
       <c r="I38" t="n">
-        <v>35.93783333333334</v>
+        <v>149.118</v>
       </c>
       <c r="J38" t="n">
-        <v>-352.6988333333334</v>
+        <v>-423.3</v>
       </c>
       <c r="K38" t="n">
-        <v>-391.68625</v>
+        <v>-386.035</v>
       </c>
       <c r="L38" t="n">
-        <v>70.16841666666666</v>
+        <v>246.065</v>
       </c>
       <c r="M38" t="n">
-        <v>-675.18475</v>
+        <v>-694.9960000000001</v>
       </c>
       <c r="N38" t="n">
-        <v>467.4448333333333</v>
+        <v>430.062</v>
       </c>
       <c r="O38" t="n">
-        <v>573.3200000000001</v>
+        <v>518.452</v>
       </c>
       <c r="P38" t="n">
-        <v>700.6065</v>
+        <v>711.7860000000001</v>
       </c>
       <c r="Q38" t="n">
-        <v>22.26425</v>
+        <v>18.237</v>
       </c>
       <c r="R38" t="n">
-        <v>18.84116666666666</v>
+        <v>15.672</v>
       </c>
       <c r="S38" t="n">
-        <v>20.24966666666667</v>
+        <v>18.538</v>
       </c>
       <c r="T38" t="n">
-        <v>9.648750000000001</v>
+        <v>6.112</v>
       </c>
       <c r="U38" t="n">
-        <v>28.16633333333334</v>
+        <v>27.456</v>
       </c>
       <c r="V38" t="n">
-        <v>248.3971666666667</v>
+        <v>247.65</v>
       </c>
       <c r="W38" t="n">
-        <v>333.7865</v>
+        <v>300.818</v>
       </c>
       <c r="X38" t="n">
-        <v>300.0774166666667</v>
+        <v>320.005</v>
       </c>
     </row>
     <row r="39">
@@ -3368,74 +3368,74 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Voll- ein- doppel- aus A</t>
+          <t>Voll- ein- halb- aus B</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>38.917</v>
+        <v>36.55214285714286</v>
       </c>
       <c r="D39" t="n">
-        <v>39.325</v>
+        <v>36.81114285714285</v>
       </c>
       <c r="E39" t="n">
-        <v>-21.164</v>
+        <v>-17.67857142857143</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.067</v>
+        <v>1.750285714285714</v>
       </c>
       <c r="G39" t="n">
-        <v>-9.732999999999999</v>
+        <v>-1.837142857142857</v>
       </c>
       <c r="H39" t="n">
-        <v>-234.922</v>
+        <v>-166.2958571428572</v>
       </c>
       <c r="I39" t="n">
-        <v>149.118</v>
+        <v>-148.081</v>
       </c>
       <c r="J39" t="n">
-        <v>-423.3</v>
+        <v>-269.501</v>
       </c>
       <c r="K39" t="n">
-        <v>-386.035</v>
+        <v>-304.3057142857143</v>
       </c>
       <c r="L39" t="n">
-        <v>246.065</v>
+        <v>-270.6174285714286</v>
       </c>
       <c r="M39" t="n">
-        <v>-694.9960000000001</v>
+        <v>-491.251</v>
       </c>
       <c r="N39" t="n">
-        <v>430.062</v>
+        <v>375.1785714285714</v>
       </c>
       <c r="O39" t="n">
-        <v>518.452</v>
+        <v>614.8082857142856</v>
       </c>
       <c r="P39" t="n">
-        <v>711.7860000000001</v>
+        <v>511.0224285714286</v>
       </c>
       <c r="Q39" t="n">
-        <v>18.237</v>
+        <v>21.43771428571429</v>
       </c>
       <c r="R39" t="n">
-        <v>15.672</v>
+        <v>19.43728571428571</v>
       </c>
       <c r="S39" t="n">
-        <v>18.538</v>
+        <v>18.40042857142857</v>
       </c>
       <c r="T39" t="n">
-        <v>6.112</v>
+        <v>10.96357142857143</v>
       </c>
       <c r="U39" t="n">
-        <v>27.456</v>
+        <v>29.04185714285714</v>
       </c>
       <c r="V39" t="n">
-        <v>247.65</v>
+        <v>241.8451428571429</v>
       </c>
       <c r="W39" t="n">
-        <v>300.818</v>
+        <v>363.649</v>
       </c>
       <c r="X39" t="n">
-        <v>320.005</v>
+        <v>261.0927142857143</v>
       </c>
     </row>
     <row r="40">
@@ -3444,74 +3444,74 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Voll- ein- halb- aus B</t>
+          <t>Voll- ein- voll- aus A</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>36.55214285714286</v>
+        <v>37.57</v>
       </c>
       <c r="D40" t="n">
-        <v>36.81114285714285</v>
+        <v>37.72</v>
       </c>
       <c r="E40" t="n">
-        <v>-17.67857142857143</v>
+        <v>-19.141</v>
       </c>
       <c r="F40" t="n">
-        <v>1.750285714285714</v>
+        <v>0.8183333333333334</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.837142857142857</v>
+        <v>-7.857333333333333</v>
       </c>
       <c r="H40" t="n">
-        <v>-166.2958571428572</v>
+        <v>-152.8063333333333</v>
       </c>
       <c r="I40" t="n">
-        <v>-148.081</v>
+        <v>148.8206666666667</v>
       </c>
       <c r="J40" t="n">
-        <v>-269.501</v>
+        <v>-394.2293333333334</v>
       </c>
       <c r="K40" t="n">
-        <v>-304.3057142857143</v>
+        <v>-265.355</v>
       </c>
       <c r="L40" t="n">
-        <v>-270.6174285714286</v>
+        <v>260.585</v>
       </c>
       <c r="M40" t="n">
-        <v>-491.251</v>
+        <v>-689.4616666666667</v>
       </c>
       <c r="N40" t="n">
-        <v>375.1785714285714</v>
+        <v>376.7353333333333</v>
       </c>
       <c r="O40" t="n">
-        <v>614.8082857142856</v>
+        <v>524.3506666666667</v>
       </c>
       <c r="P40" t="n">
-        <v>511.0224285714286</v>
+        <v>720.4110000000001</v>
       </c>
       <c r="Q40" t="n">
-        <v>21.43771428571429</v>
+        <v>19.419</v>
       </c>
       <c r="R40" t="n">
-        <v>19.43728571428571</v>
+        <v>16.74333333333334</v>
       </c>
       <c r="S40" t="n">
-        <v>18.40042857142857</v>
+        <v>16.94133333333333</v>
       </c>
       <c r="T40" t="n">
-        <v>10.96357142857143</v>
+        <v>6.036333333333334</v>
       </c>
       <c r="U40" t="n">
-        <v>29.04185714285714</v>
+        <v>30.00833333333334</v>
       </c>
       <c r="V40" t="n">
-        <v>241.8451428571429</v>
+        <v>241.6536666666667</v>
       </c>
       <c r="W40" t="n">
-        <v>363.649</v>
+        <v>283.512</v>
       </c>
       <c r="X40" t="n">
-        <v>261.0927142857143</v>
+        <v>302.9816666666666</v>
       </c>
     </row>
     <row r="41">
@@ -3520,74 +3520,74 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus A</t>
+          <t>Voll- ein- halb- aus C</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>37.57</v>
+        <v>35.57899999999999</v>
       </c>
       <c r="D41" t="n">
-        <v>37.72</v>
+        <v>36.006</v>
       </c>
       <c r="E41" t="n">
-        <v>-19.141</v>
+        <v>-16.3615</v>
       </c>
       <c r="F41" t="n">
-        <v>0.8183333333333334</v>
+        <v>2.287</v>
       </c>
       <c r="G41" t="n">
-        <v>-7.857333333333333</v>
+        <v>-5.0425</v>
       </c>
       <c r="H41" t="n">
-        <v>-152.8063333333333</v>
+        <v>-193.664</v>
       </c>
       <c r="I41" t="n">
-        <v>148.8206666666667</v>
+        <v>-106.441</v>
       </c>
       <c r="J41" t="n">
-        <v>-394.2293333333334</v>
+        <v>-210.1095</v>
       </c>
       <c r="K41" t="n">
-        <v>-265.355</v>
+        <v>-361.5445</v>
       </c>
       <c r="L41" t="n">
-        <v>260.585</v>
+        <v>-200.397</v>
       </c>
       <c r="M41" t="n">
-        <v>-689.4616666666667</v>
+        <v>-390.9055</v>
       </c>
       <c r="N41" t="n">
-        <v>376.7353333333333</v>
+        <v>429.688</v>
       </c>
       <c r="O41" t="n">
-        <v>524.3506666666667</v>
+        <v>589.9005</v>
       </c>
       <c r="P41" t="n">
-        <v>720.4110000000001</v>
+        <v>486.898</v>
       </c>
       <c r="Q41" t="n">
-        <v>19.419</v>
+        <v>23.2275</v>
       </c>
       <c r="R41" t="n">
-        <v>16.74333333333334</v>
+        <v>21.202</v>
       </c>
       <c r="S41" t="n">
-        <v>16.94133333333333</v>
+        <v>18.3185</v>
       </c>
       <c r="T41" t="n">
-        <v>6.036333333333334</v>
+        <v>8.118500000000001</v>
       </c>
       <c r="U41" t="n">
-        <v>30.00833333333334</v>
+        <v>30.281</v>
       </c>
       <c r="V41" t="n">
-        <v>241.6536666666667</v>
+        <v>271.813</v>
       </c>
       <c r="W41" t="n">
-        <v>283.512</v>
+        <v>340.7965</v>
       </c>
       <c r="X41" t="n">
-        <v>302.9816666666666</v>
+        <v>276.106</v>
       </c>
     </row>
     <row r="42">
@@ -3596,74 +3596,74 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Voll- ein- halb- aus C</t>
+          <t>Voll- ein- voll- aus C</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>35.57899999999999</v>
+        <v>36.96</v>
       </c>
       <c r="D42" t="n">
-        <v>36.006</v>
+        <v>37.11533333333333</v>
       </c>
       <c r="E42" t="n">
-        <v>-16.3615</v>
+        <v>-19.18533333333333</v>
       </c>
       <c r="F42" t="n">
-        <v>2.287</v>
+        <v>1.532333333333333</v>
       </c>
       <c r="G42" t="n">
-        <v>-5.0425</v>
+        <v>-4.649</v>
       </c>
       <c r="H42" t="n">
-        <v>-193.664</v>
+        <v>-234.7186666666666</v>
       </c>
       <c r="I42" t="n">
-        <v>-106.441</v>
+        <v>51.97133333333333</v>
       </c>
       <c r="J42" t="n">
-        <v>-210.1095</v>
+        <v>-365.91</v>
       </c>
       <c r="K42" t="n">
-        <v>-361.5445</v>
+        <v>-412.3086666666666</v>
       </c>
       <c r="L42" t="n">
-        <v>-200.397</v>
+        <v>96.87366666666667</v>
       </c>
       <c r="M42" t="n">
-        <v>-390.9055</v>
+        <v>-644.6663333333335</v>
       </c>
       <c r="N42" t="n">
-        <v>429.688</v>
+        <v>434.0596666666667</v>
       </c>
       <c r="O42" t="n">
-        <v>589.9005</v>
+        <v>522.3663333333334</v>
       </c>
       <c r="P42" t="n">
-        <v>486.898</v>
+        <v>668.6133333333333</v>
       </c>
       <c r="Q42" t="n">
-        <v>23.2275</v>
+        <v>19.804</v>
       </c>
       <c r="R42" t="n">
-        <v>21.202</v>
+        <v>16.885</v>
       </c>
       <c r="S42" t="n">
-        <v>18.3185</v>
+        <v>18.95833333333333</v>
       </c>
       <c r="T42" t="n">
-        <v>8.118500000000001</v>
+        <v>6.530666666666666</v>
       </c>
       <c r="U42" t="n">
-        <v>30.281</v>
+        <v>28.20633333333333</v>
       </c>
       <c r="V42" t="n">
-        <v>271.813</v>
+        <v>231.889</v>
       </c>
       <c r="W42" t="n">
-        <v>340.7965</v>
+        <v>315.9226666666667</v>
       </c>
       <c r="X42" t="n">
-        <v>276.106</v>
+        <v>307.771</v>
       </c>
     </row>
     <row r="43">
@@ -3672,74 +3672,74 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Voll- ein- voll- aus C</t>
+          <t>Voll- ein 1 3/4 Salto vw C</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>36.96</v>
+        <v>29.22833333333334</v>
       </c>
       <c r="D43" t="n">
-        <v>37.11533333333333</v>
+        <v>29.149</v>
       </c>
       <c r="E43" t="n">
-        <v>-19.18533333333333</v>
+        <v>-15.22433333333333</v>
       </c>
       <c r="F43" t="n">
-        <v>1.532333333333333</v>
+        <v>-1.255</v>
       </c>
       <c r="G43" t="n">
-        <v>-4.649</v>
+        <v>-1.538333333333333</v>
       </c>
       <c r="H43" t="n">
-        <v>-234.7186666666666</v>
+        <v>95.19566666666667</v>
       </c>
       <c r="I43" t="n">
-        <v>51.97133333333333</v>
+        <v>-223.5676666666667</v>
       </c>
       <c r="J43" t="n">
-        <v>-365.91</v>
+        <v>139.9815</v>
       </c>
       <c r="K43" t="n">
-        <v>-412.3086666666666</v>
+        <v>190.6551666666667</v>
       </c>
       <c r="L43" t="n">
-        <v>96.87366666666667</v>
+        <v>-430.3043333333333</v>
       </c>
       <c r="M43" t="n">
-        <v>-644.6663333333335</v>
+        <v>292.468</v>
       </c>
       <c r="N43" t="n">
-        <v>434.0596666666667</v>
+        <v>348.5503333333334</v>
       </c>
       <c r="O43" t="n">
-        <v>522.3663333333334</v>
+        <v>505.584</v>
       </c>
       <c r="P43" t="n">
-        <v>668.6133333333333</v>
+        <v>333.5115</v>
       </c>
       <c r="Q43" t="n">
-        <v>19.804</v>
+        <v>23.06016666666666</v>
       </c>
       <c r="R43" t="n">
-        <v>16.885</v>
+        <v>19.757</v>
       </c>
       <c r="S43" t="n">
-        <v>18.95833333333333</v>
+        <v>15.19483333333333</v>
       </c>
       <c r="T43" t="n">
-        <v>6.530666666666666</v>
+        <v>7.741333333333333</v>
       </c>
       <c r="U43" t="n">
-        <v>28.20633333333333</v>
+        <v>24.45033333333333</v>
       </c>
       <c r="V43" t="n">
-        <v>231.889</v>
+        <v>230.0946666666667</v>
       </c>
       <c r="W43" t="n">
-        <v>315.9226666666667</v>
+        <v>193.8886666666667</v>
       </c>
       <c r="X43" t="n">
-        <v>307.771</v>
+        <v>200.9821666666667</v>
       </c>
     </row>
     <row r="44">
@@ -3748,74 +3748,74 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Voll- ein 1 3/4 Salto vw C</t>
+          <t>1 3/4 Salto vw C</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>29.22833333333334</v>
+        <v>26.8828</v>
       </c>
       <c r="D44" t="n">
-        <v>29.149</v>
+        <v>26.93</v>
       </c>
       <c r="E44" t="n">
-        <v>-15.22433333333333</v>
+        <v>-14.5824</v>
       </c>
       <c r="F44" t="n">
-        <v>-1.255</v>
+        <v>0.0854</v>
       </c>
       <c r="G44" t="n">
-        <v>-1.538333333333333</v>
+        <v>0.9917999999999999</v>
       </c>
       <c r="H44" t="n">
-        <v>95.19566666666667</v>
+        <v>6.622</v>
       </c>
       <c r="I44" t="n">
-        <v>-223.5676666666667</v>
+        <v>-342.1744</v>
       </c>
       <c r="J44" t="n">
-        <v>139.9815</v>
+        <v>1.2608</v>
       </c>
       <c r="K44" t="n">
-        <v>190.6551666666667</v>
+        <v>17.9002</v>
       </c>
       <c r="L44" t="n">
-        <v>-430.3043333333333</v>
+        <v>-661.8158000000001</v>
       </c>
       <c r="M44" t="n">
-        <v>292.468</v>
+        <v>24.689</v>
       </c>
       <c r="N44" t="n">
-        <v>348.5503333333334</v>
+        <v>38.9594</v>
       </c>
       <c r="O44" t="n">
-        <v>505.584</v>
+        <v>673.4341999999999</v>
       </c>
       <c r="P44" t="n">
-        <v>333.5115</v>
+        <v>60.08000000000001</v>
       </c>
       <c r="Q44" t="n">
-        <v>23.06016666666666</v>
+        <v>25.9652</v>
       </c>
       <c r="R44" t="n">
-        <v>19.757</v>
+        <v>22.9034</v>
       </c>
       <c r="S44" t="n">
-        <v>15.19483333333333</v>
+        <v>18.4732</v>
       </c>
       <c r="T44" t="n">
-        <v>7.741333333333333</v>
+        <v>1.9258</v>
       </c>
       <c r="U44" t="n">
-        <v>24.45033333333333</v>
+        <v>24.0882</v>
       </c>
       <c r="V44" t="n">
-        <v>230.0946666666667</v>
+        <v>19.041</v>
       </c>
       <c r="W44" t="n">
-        <v>193.8886666666667</v>
+        <v>200.656</v>
       </c>
       <c r="X44" t="n">
-        <v>200.9821666666667</v>
+        <v>26.8358</v>
       </c>
     </row>
     <row r="45">
@@ -3824,74 +3824,74 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1 3/4 Salto vw C</t>
+          <t>Triffis B</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>26.8828</v>
+        <v>45.343</v>
       </c>
       <c r="D45" t="n">
-        <v>26.93</v>
+        <v>45.5032</v>
       </c>
       <c r="E45" t="n">
-        <v>-14.5824</v>
+        <v>-27.2924</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0854</v>
+        <v>6.956999999999999</v>
       </c>
       <c r="G45" t="n">
-        <v>0.9917999999999999</v>
+        <v>-2.6092</v>
       </c>
       <c r="H45" t="n">
-        <v>6.622</v>
+        <v>-98.2574</v>
       </c>
       <c r="I45" t="n">
-        <v>-342.1744</v>
+        <v>-368.478</v>
       </c>
       <c r="J45" t="n">
-        <v>1.2608</v>
+        <v>-94.74039999999999</v>
       </c>
       <c r="K45" t="n">
-        <v>17.9002</v>
+        <v>-195.0148</v>
       </c>
       <c r="L45" t="n">
-        <v>-661.8158000000001</v>
+        <v>-732.9498000000001</v>
       </c>
       <c r="M45" t="n">
-        <v>24.689</v>
+        <v>-188.6016</v>
       </c>
       <c r="N45" t="n">
-        <v>38.9594</v>
+        <v>316.7212000000001</v>
       </c>
       <c r="O45" t="n">
-        <v>673.4341999999999</v>
+        <v>982.6779999999999</v>
       </c>
       <c r="P45" t="n">
-        <v>60.08000000000001</v>
+        <v>278.2516</v>
       </c>
       <c r="Q45" t="n">
-        <v>25.9652</v>
+        <v>23.2562</v>
       </c>
       <c r="R45" t="n">
-        <v>22.9034</v>
+        <v>21.3198</v>
       </c>
       <c r="S45" t="n">
-        <v>18.4732</v>
+        <v>24.5062</v>
       </c>
       <c r="T45" t="n">
-        <v>1.9258</v>
+        <v>9.521800000000001</v>
       </c>
       <c r="U45" t="n">
-        <v>24.0882</v>
+        <v>30.622</v>
       </c>
       <c r="V45" t="n">
-        <v>19.041</v>
+        <v>163.7492</v>
       </c>
       <c r="W45" t="n">
-        <v>200.656</v>
+        <v>431.4264</v>
       </c>
       <c r="X45" t="n">
-        <v>26.8358</v>
+        <v>173.0902</v>
       </c>
     </row>
     <row r="46">
@@ -3900,74 +3900,74 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Triffis B</t>
+          <t>Halb- ein- halb- aus B</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>45.343</v>
+        <v>35.128</v>
       </c>
       <c r="D46" t="n">
-        <v>45.5032</v>
+        <v>34.865</v>
       </c>
       <c r="E46" t="n">
-        <v>-27.2924</v>
+        <v>-16.819</v>
       </c>
       <c r="F46" t="n">
-        <v>6.956999999999999</v>
+        <v>4.405</v>
       </c>
       <c r="G46" t="n">
-        <v>-2.6092</v>
+        <v>-2.158</v>
       </c>
       <c r="H46" t="n">
-        <v>-98.2574</v>
+        <v>-125.656</v>
       </c>
       <c r="I46" t="n">
-        <v>-368.478</v>
+        <v>-85.64200000000001</v>
       </c>
       <c r="J46" t="n">
-        <v>-94.74039999999999</v>
+        <v>-167.185</v>
       </c>
       <c r="K46" t="n">
-        <v>-195.0148</v>
+        <v>-215.313</v>
       </c>
       <c r="L46" t="n">
-        <v>-732.9498000000001</v>
+        <v>-143.538</v>
       </c>
       <c r="M46" t="n">
-        <v>-188.6016</v>
+        <v>-286.615</v>
       </c>
       <c r="N46" t="n">
-        <v>316.7212000000001</v>
+        <v>322.824</v>
       </c>
       <c r="O46" t="n">
-        <v>982.6779999999999</v>
+        <v>575.2809999999999</v>
       </c>
       <c r="P46" t="n">
-        <v>278.2516</v>
+        <v>370.702</v>
       </c>
       <c r="Q46" t="n">
-        <v>23.2562</v>
+        <v>21.684</v>
       </c>
       <c r="R46" t="n">
-        <v>21.3198</v>
+        <v>18.348</v>
       </c>
       <c r="S46" t="n">
-        <v>24.5062</v>
+        <v>18.576</v>
       </c>
       <c r="T46" t="n">
-        <v>9.521800000000001</v>
+        <v>9.635</v>
       </c>
       <c r="U46" t="n">
-        <v>30.622</v>
+        <v>28.464</v>
       </c>
       <c r="V46" t="n">
-        <v>163.7492</v>
+        <v>210.182</v>
       </c>
       <c r="W46" t="n">
-        <v>431.4264</v>
+        <v>379.163</v>
       </c>
       <c r="X46" t="n">
-        <v>173.0902</v>
+        <v>200.306</v>
       </c>
     </row>
     <row r="47">
@@ -3976,74 +3976,74 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Halb- ein- halb- aus B</t>
+          <t>Halb- ein- halb- aus C</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>35.128</v>
+        <v>36.678</v>
       </c>
       <c r="D47" t="n">
-        <v>34.865</v>
+        <v>36.472</v>
       </c>
       <c r="E47" t="n">
-        <v>-16.819</v>
+        <v>-17.34</v>
       </c>
       <c r="F47" t="n">
-        <v>4.405</v>
+        <v>3.319</v>
       </c>
       <c r="G47" t="n">
-        <v>-2.158</v>
+        <v>-4.671</v>
       </c>
       <c r="H47" t="n">
-        <v>-125.656</v>
+        <v>-120.127</v>
       </c>
       <c r="I47" t="n">
-        <v>-85.64200000000001</v>
+        <v>-97.44</v>
       </c>
       <c r="J47" t="n">
-        <v>-167.185</v>
+        <v>-155.547</v>
       </c>
       <c r="K47" t="n">
-        <v>-215.313</v>
+        <v>-205.367</v>
       </c>
       <c r="L47" t="n">
-        <v>-143.538</v>
+        <v>-165.06</v>
       </c>
       <c r="M47" t="n">
-        <v>-286.615</v>
+        <v>-265.518</v>
       </c>
       <c r="N47" t="n">
-        <v>322.824</v>
+        <v>297.207</v>
       </c>
       <c r="O47" t="n">
-        <v>575.2809999999999</v>
+        <v>584.437</v>
       </c>
       <c r="P47" t="n">
-        <v>370.702</v>
+        <v>366.502</v>
       </c>
       <c r="Q47" t="n">
-        <v>21.684</v>
+        <v>23.556</v>
       </c>
       <c r="R47" t="n">
-        <v>18.348</v>
+        <v>20.994</v>
       </c>
       <c r="S47" t="n">
-        <v>18.576</v>
+        <v>22.72</v>
       </c>
       <c r="T47" t="n">
-        <v>9.635</v>
+        <v>8.277999999999999</v>
       </c>
       <c r="U47" t="n">
-        <v>28.464</v>
+        <v>28.907</v>
       </c>
       <c r="V47" t="n">
-        <v>210.182</v>
+        <v>208.485</v>
       </c>
       <c r="W47" t="n">
-        <v>379.163</v>
+        <v>393.7380000000001</v>
       </c>
       <c r="X47" t="n">
-        <v>200.306</v>
+        <v>199.733</v>
       </c>
     </row>
     <row r="48">
@@ -4052,74 +4052,74 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Halb- ein- halb- aus C</t>
+          <t>Halb- ein- Rudy- aus B</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>36.678</v>
+        <v>39.131</v>
       </c>
       <c r="D48" t="n">
-        <v>36.472</v>
+        <v>39.188</v>
       </c>
       <c r="E48" t="n">
-        <v>-17.34</v>
+        <v>-19.987</v>
       </c>
       <c r="F48" t="n">
-        <v>3.319</v>
+        <v>2.927</v>
       </c>
       <c r="G48" t="n">
-        <v>-4.671</v>
+        <v>-1.328</v>
       </c>
       <c r="H48" t="n">
-        <v>-120.127</v>
+        <v>-195.663</v>
       </c>
       <c r="I48" t="n">
-        <v>-97.44</v>
+        <v>-3.235</v>
       </c>
       <c r="J48" t="n">
-        <v>-155.547</v>
+        <v>-361.304</v>
       </c>
       <c r="K48" t="n">
-        <v>-205.367</v>
+        <v>-368.043</v>
       </c>
       <c r="L48" t="n">
-        <v>-165.06</v>
+        <v>-4.551</v>
       </c>
       <c r="M48" t="n">
-        <v>-265.518</v>
+        <v>-680.7089999999999</v>
       </c>
       <c r="N48" t="n">
-        <v>297.207</v>
+        <v>477.2430000000001</v>
       </c>
       <c r="O48" t="n">
-        <v>584.437</v>
+        <v>571.381</v>
       </c>
       <c r="P48" t="n">
-        <v>366.502</v>
+        <v>696.701</v>
       </c>
       <c r="Q48" t="n">
-        <v>23.556</v>
+        <v>22.256</v>
       </c>
       <c r="R48" t="n">
-        <v>20.994</v>
+        <v>18.544</v>
       </c>
       <c r="S48" t="n">
-        <v>22.72</v>
+        <v>19.263</v>
       </c>
       <c r="T48" t="n">
-        <v>8.277999999999999</v>
+        <v>13.373</v>
       </c>
       <c r="U48" t="n">
-        <v>28.907</v>
+        <v>29.654</v>
       </c>
       <c r="V48" t="n">
-        <v>208.485</v>
+        <v>247.62</v>
       </c>
       <c r="W48" t="n">
-        <v>393.7380000000001</v>
+        <v>354.3</v>
       </c>
       <c r="X48" t="n">
-        <v>199.733</v>
+        <v>291.56</v>
       </c>
     </row>
     <row r="49">
@@ -4128,74 +4128,74 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Halb- ein- Rudy- aus B</t>
+          <t>Schraubensalto C</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>39.131</v>
+        <v>17.13769387755102</v>
       </c>
       <c r="D49" t="n">
-        <v>39.188</v>
+        <v>17.03928571428571</v>
       </c>
       <c r="E49" t="n">
-        <v>-19.987</v>
+        <v>-2.480428571428572</v>
       </c>
       <c r="F49" t="n">
-        <v>2.927</v>
+        <v>-0.7355306122448979</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.328</v>
+        <v>5.578591836734695</v>
       </c>
       <c r="H49" t="n">
-        <v>-195.663</v>
+        <v>41.7034693877551</v>
       </c>
       <c r="I49" t="n">
-        <v>-3.235</v>
+        <v>93.78261224489798</v>
       </c>
       <c r="J49" t="n">
-        <v>-361.304</v>
+        <v>211.2369591836735</v>
       </c>
       <c r="K49" t="n">
-        <v>-368.043</v>
+        <v>78.98699999999999</v>
       </c>
       <c r="L49" t="n">
-        <v>-4.551</v>
+        <v>175.5836938775511</v>
       </c>
       <c r="M49" t="n">
-        <v>-680.7089999999999</v>
+        <v>395.8561224489796</v>
       </c>
       <c r="N49" t="n">
-        <v>477.2430000000001</v>
+        <v>162.7044489795918</v>
       </c>
       <c r="O49" t="n">
-        <v>571.381</v>
+        <v>280.2916122448979</v>
       </c>
       <c r="P49" t="n">
-        <v>696.701</v>
+        <v>400.5705918367346</v>
       </c>
       <c r="Q49" t="n">
-        <v>22.256</v>
+        <v>23.09702040816326</v>
       </c>
       <c r="R49" t="n">
-        <v>18.544</v>
+        <v>20.62551020408163</v>
       </c>
       <c r="S49" t="n">
-        <v>19.263</v>
+        <v>10.63020408163265</v>
       </c>
       <c r="T49" t="n">
-        <v>13.373</v>
+        <v>2.629204081632653</v>
       </c>
       <c r="U49" t="n">
-        <v>29.654</v>
+        <v>24.45461224489796</v>
       </c>
       <c r="V49" t="n">
-        <v>247.62</v>
+        <v>106.5022244897959</v>
       </c>
       <c r="W49" t="n">
-        <v>354.3</v>
+        <v>129.5556326530612</v>
       </c>
       <c r="X49" t="n">
-        <v>291.56</v>
+        <v>162.0674693877551</v>
       </c>
     </row>
     <row r="50">
@@ -4204,74 +4204,74 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Schraubensalto C</t>
+          <t>Bauchsprung</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17.13769387755102</v>
+        <v>11.95702702702703</v>
       </c>
       <c r="D50" t="n">
-        <v>17.03928571428571</v>
+        <v>11.32617567567567</v>
       </c>
       <c r="E50" t="n">
-        <v>-2.480428571428572</v>
+        <v>4.756094594594595</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.7355306122448979</v>
+        <v>-0.1839594594594595</v>
       </c>
       <c r="G50" t="n">
-        <v>5.578591836734695</v>
+        <v>7.233013513513512</v>
       </c>
       <c r="H50" t="n">
-        <v>41.7034693877551</v>
+        <v>-2.007094594594595</v>
       </c>
       <c r="I50" t="n">
-        <v>93.78261224489798</v>
+        <v>-21.71147297297297</v>
       </c>
       <c r="J50" t="n">
-        <v>211.2369591836735</v>
+        <v>-4.42981081081081</v>
       </c>
       <c r="K50" t="n">
-        <v>78.98699999999999</v>
+        <v>-3.847472972972974</v>
       </c>
       <c r="L50" t="n">
-        <v>175.5836938775511</v>
+        <v>-38.9775</v>
       </c>
       <c r="M50" t="n">
-        <v>395.8561224489796</v>
+        <v>-8.317594594594594</v>
       </c>
       <c r="N50" t="n">
-        <v>162.7044489795918</v>
+        <v>21.71535135135135</v>
       </c>
       <c r="O50" t="n">
-        <v>280.2916122448979</v>
+        <v>119.7072567567568</v>
       </c>
       <c r="P50" t="n">
-        <v>400.5705918367346</v>
+        <v>35.68600000000001</v>
       </c>
       <c r="Q50" t="n">
-        <v>23.09702040816326</v>
+        <v>24.26571621621622</v>
       </c>
       <c r="R50" t="n">
-        <v>20.62551020408163</v>
+        <v>21.49163513513514</v>
       </c>
       <c r="S50" t="n">
-        <v>10.63020408163265</v>
+        <v>15.04294594594595</v>
       </c>
       <c r="T50" t="n">
-        <v>2.629204081632653</v>
+        <v>1.200878378378379</v>
       </c>
       <c r="U50" t="n">
-        <v>24.45461224489796</v>
+        <v>19.41366216216217</v>
       </c>
       <c r="V50" t="n">
-        <v>106.5022244897959</v>
+        <v>12.90618918918919</v>
       </c>
       <c r="W50" t="n">
-        <v>129.5556326530612</v>
+        <v>71.9982972972973</v>
       </c>
       <c r="X50" t="n">
-        <v>162.0674693877551</v>
+        <v>19.88351351351351</v>
       </c>
     </row>
     <row r="51">
@@ -4280,149 +4280,73 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bauchsprung</t>
+          <t>Von Bauch in Stand</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>11.95702702702703</v>
+        <v>12.73906756756757</v>
       </c>
       <c r="D51" t="n">
-        <v>11.32617567567567</v>
+        <v>13.21222972972973</v>
       </c>
       <c r="E51" t="n">
-        <v>4.756094594594595</v>
+        <v>6.384635135135134</v>
       </c>
       <c r="F51" t="n">
-        <v>-0.1839594594594595</v>
+        <v>-0.01454054054054054</v>
       </c>
       <c r="G51" t="n">
-        <v>7.233013513513512</v>
+        <v>6.474905405405406</v>
       </c>
       <c r="H51" t="n">
-        <v>-2.007094594594595</v>
+        <v>2.209797297297297</v>
       </c>
       <c r="I51" t="n">
-        <v>-21.71147297297297</v>
+        <v>22.75035135135135</v>
       </c>
       <c r="J51" t="n">
-        <v>-4.42981081081081</v>
+        <v>3.928756756756756</v>
       </c>
       <c r="K51" t="n">
-        <v>-3.847472972972974</v>
+        <v>3.957702702702702</v>
       </c>
       <c r="L51" t="n">
-        <v>-38.9775</v>
+        <v>38.25474324324325</v>
       </c>
       <c r="M51" t="n">
-        <v>-8.317594594594594</v>
+        <v>7.01945945945946</v>
       </c>
       <c r="N51" t="n">
-        <v>21.71535135135135</v>
+        <v>25.20467567567567</v>
       </c>
       <c r="O51" t="n">
-        <v>119.7072567567568</v>
+        <v>83.52685135135135</v>
       </c>
       <c r="P51" t="n">
-        <v>35.68600000000001</v>
+        <v>40.98166216216216</v>
       </c>
       <c r="Q51" t="n">
-        <v>24.26571621621622</v>
+        <v>24.26547297297298</v>
       </c>
       <c r="R51" t="n">
-        <v>21.49163513513514</v>
+        <v>24.46771621621621</v>
       </c>
       <c r="S51" t="n">
-        <v>15.04294594594595</v>
+        <v>16.66471621621622</v>
       </c>
       <c r="T51" t="n">
-        <v>1.200878378378379</v>
+        <v>1.57622972972973</v>
       </c>
       <c r="U51" t="n">
-        <v>19.41366216216217</v>
+        <v>17.78168918918919</v>
       </c>
       <c r="V51" t="n">
-        <v>12.90618918918919</v>
+        <v>15.6312027027027</v>
       </c>
       <c r="W51" t="n">
-        <v>71.9982972972973</v>
+        <v>64.54325675675676</v>
       </c>
       <c r="X51" t="n">
-        <v>19.88351351351351</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Von Bauch in Stand</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>12.73906756756757</v>
-      </c>
-      <c r="D52" t="n">
-        <v>13.21222972972973</v>
-      </c>
-      <c r="E52" t="n">
-        <v>6.384635135135134</v>
-      </c>
-      <c r="F52" t="n">
-        <v>-0.01454054054054054</v>
-      </c>
-      <c r="G52" t="n">
-        <v>6.474905405405406</v>
-      </c>
-      <c r="H52" t="n">
-        <v>2.209797297297297</v>
-      </c>
-      <c r="I52" t="n">
-        <v>22.75035135135135</v>
-      </c>
-      <c r="J52" t="n">
-        <v>3.928756756756756</v>
-      </c>
-      <c r="K52" t="n">
-        <v>3.957702702702702</v>
-      </c>
-      <c r="L52" t="n">
-        <v>38.25474324324325</v>
-      </c>
-      <c r="M52" t="n">
-        <v>7.01945945945946</v>
-      </c>
-      <c r="N52" t="n">
-        <v>25.20467567567567</v>
-      </c>
-      <c r="O52" t="n">
-        <v>83.52685135135135</v>
-      </c>
-      <c r="P52" t="n">
-        <v>40.98166216216216</v>
-      </c>
-      <c r="Q52" t="n">
-        <v>24.26547297297298</v>
-      </c>
-      <c r="R52" t="n">
-        <v>24.46771621621621</v>
-      </c>
-      <c r="S52" t="n">
-        <v>16.66471621621622</v>
-      </c>
-      <c r="T52" t="n">
-        <v>1.57622972972973</v>
-      </c>
-      <c r="U52" t="n">
-        <v>17.78168918918919</v>
-      </c>
-      <c r="V52" t="n">
-        <v>15.6312027027027</v>
-      </c>
-      <c r="W52" t="n">
-        <v>64.54325675675676</v>
-      </c>
-      <c r="X52" t="n">
         <v>21.76814864864865</v>
       </c>
     </row>

</xml_diff>